<commit_message>
importing now returns success even with empty xls rows
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/simple_test.xlsx
+++ b/spec/fixtures/files/simple_test.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Serial No</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>ALPHA GROUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -498,10 +501,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,6 +591,22 @@
         <v>19</v>
       </c>
     </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="9"/>
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>